<commit_message>
change raw materials dataset
 raw materials 02
</commit_message>
<xml_diff>
--- a/Dataset/Component-raw mat/raw mat data set.xlsx
+++ b/Dataset/Component-raw mat/raw mat data set.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akish\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akish\Documents\GitHub\research\House-Plan-Master\Dataset\Component-raw mat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF0B98FD-3144-4A34-ACE1-109C38ABA105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2B52F8-4CCC-41EC-B5BD-03033E5B939D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC4DFFEB-EC04-477D-98D2-6D536FB84C59}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t xml:space="preserve">cement </t>
   </si>
@@ -43,18 +43,9 @@
     <t>sand</t>
   </si>
   <si>
-    <t>stone</t>
-  </si>
-  <si>
-    <t>matel</t>
-  </si>
-  <si>
     <t>steel</t>
   </si>
   <si>
-    <t>Sure feet</t>
-  </si>
-  <si>
     <t>thickness</t>
   </si>
   <si>
@@ -64,12 +55,6 @@
     <t>1 sq ft</t>
   </si>
   <si>
-    <t>0.4 bag</t>
-  </si>
-  <si>
-    <t>400 bag</t>
-  </si>
-  <si>
     <t>1.8 cft</t>
   </si>
   <si>
@@ -94,9 +79,6 @@
     <t>2000 sq ft</t>
   </si>
   <si>
-    <t>800 bag</t>
-  </si>
-  <si>
     <t>3600 ctf</t>
   </si>
   <si>
@@ -118,7 +100,118 @@
     <t>2000kg</t>
   </si>
   <si>
-    <t>24000kg</t>
+    <t>2400kg</t>
+  </si>
+  <si>
+    <t>3600kg</t>
+  </si>
+  <si>
+    <t>2500 sq ft</t>
+  </si>
+  <si>
+    <t>Squre feet</t>
+  </si>
+  <si>
+    <t>10000kg</t>
+  </si>
+  <si>
+    <t>3000 sq ft</t>
+  </si>
+  <si>
+    <t>3500 sq ft</t>
+  </si>
+  <si>
+    <t>12000kg</t>
+  </si>
+  <si>
+    <t>14000kg</t>
+  </si>
+  <si>
+    <t>900 cft</t>
+  </si>
+  <si>
+    <t>1080 cft</t>
+  </si>
+  <si>
+    <t>1620 cft</t>
+  </si>
+  <si>
+    <t>4500 cft</t>
+  </si>
+  <si>
+    <t>5400 cft</t>
+  </si>
+  <si>
+    <t>6300 cft</t>
+  </si>
+  <si>
+    <t>725 sqft</t>
+  </si>
+  <si>
+    <t>870 sqft</t>
+  </si>
+  <si>
+    <t>1305 sqft</t>
+  </si>
+  <si>
+    <t>3625 sqft</t>
+  </si>
+  <si>
+    <t>4350 sqft</t>
+  </si>
+  <si>
+    <t>5075 sqft</t>
+  </si>
+  <si>
+    <t>76 bag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38000 bag </t>
+  </si>
+  <si>
+    <t>45600  bag</t>
+  </si>
+  <si>
+    <t>68400   bag</t>
+  </si>
+  <si>
+    <t>76000 bag</t>
+  </si>
+  <si>
+    <t>152000 bag</t>
+  </si>
+  <si>
+    <t>190000 bag</t>
+  </si>
+  <si>
+    <t>228000 bag</t>
+  </si>
+  <si>
+    <t>266000 bag</t>
+  </si>
+  <si>
+    <t>95 bag</t>
+  </si>
+  <si>
+    <t>47500 bag</t>
+  </si>
+  <si>
+    <t>57000  bag</t>
+  </si>
+  <si>
+    <t>85500   bag</t>
+  </si>
+  <si>
+    <t>95000 bag</t>
+  </si>
+  <si>
+    <t>237500 bag</t>
+  </si>
+  <si>
+    <t>285000 bag</t>
+  </si>
+  <si>
+    <t>332500 bag</t>
   </si>
 </sst>
 </file>
@@ -142,7 +235,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -150,12 +243,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708C0902-5678-43C5-A08B-94184A76CBA9}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,120 +679,393 @@
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" s="6">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="C8" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
+      <c r="D8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="7">
+        <v>6</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="7">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="7">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="7">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="C19" s="7">
+        <v>6</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="C20" s="7">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
+      <c r="C21" s="8">
+        <v>6</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>